<commit_message>
value from sim isf agent memory
</commit_message>
<xml_diff>
--- a/src/main/java/safe_rl/runners/trading/results/scen_res_DayId[year=24, month=0, day=0, region=se3].xlsx
+++ b/src/main/java/safe_rl/runners/trading/results/scen_res_DayId[year=24, month=0, day=0, region=se3].xlsx
@@ -47,7 +47,7 @@
     <t>G2V</t>
   </si>
   <si>
-    <t>-2.7</t>
+    <t>-5.7</t>
   </si>
   <si>
     <t>-0</t>
@@ -56,13 +56,13 @@
     <t>V2G</t>
   </si>
   <si>
-    <t>-0.1</t>
+    <t>-0.3</t>
   </si>
   <si>
     <t>-0.5</t>
   </si>
   <si>
-    <t>-0.6</t>
+    <t>-0.8</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
x-ticks enligt riktigt tid fromToHout
</commit_message>
<xml_diff>
--- a/src/main/java/safe_rl/runners/trading/results/scen_res_DayId[year=24, month=0, day=0, region=se3].xlsx
+++ b/src/main/java/safe_rl/runners/trading/results/scen_res_DayId[year=24, month=0, day=0, region=se3].xlsx
@@ -47,7 +47,7 @@
     <t>G2V</t>
   </si>
   <si>
-    <t>-5.7</t>
+    <t>-5.9</t>
   </si>
   <si>
     <t>-0</t>
@@ -56,13 +56,13 @@
     <t>V2G</t>
   </si>
   <si>
-    <t>-0.3</t>
+    <t>0.4</t>
   </si>
   <si>
     <t>-0.5</t>
   </si>
   <si>
-    <t>-0.8</t>
+    <t>-0.09999999999999998</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
START_SOC och DELTA_SOC isf SOC_FINAL
</commit_message>
<xml_diff>
--- a/src/main/java/safe_rl/runners/trading/results/scen_res_DayId[year=24, month=0, day=0, region=se3].xlsx
+++ b/src/main/java/safe_rl/runners/trading/results/scen_res_DayId[year=24, month=0, day=0, region=se3].xlsx
@@ -56,13 +56,13 @@
     <t>V2G</t>
   </si>
   <si>
-    <t>0.4</t>
+    <t>0.2</t>
   </si>
   <si>
     <t>-0.5</t>
   </si>
   <si>
-    <t>-0.09999999999999998</t>
+    <t>-0.3</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
soc delta i settings  socTermMin som fcn
</commit_message>
<xml_diff>
--- a/src/main/java/safe_rl/runners/trading/results/scen_res_DayId[year=24, month=0, day=0, region=se3].xlsx
+++ b/src/main/java/safe_rl/runners/trading/results/scen_res_DayId[year=24, month=0, day=0, region=se3].xlsx
@@ -47,7 +47,7 @@
     <t>G2V</t>
   </si>
   <si>
-    <t>-5.9</t>
+    <t>-5.3</t>
   </si>
   <si>
     <t>-0</t>
@@ -56,13 +56,13 @@
     <t>V2G</t>
   </si>
   <si>
-    <t>0.2</t>
+    <t>3.9</t>
   </si>
   <si>
     <t>-0.5</t>
   </si>
   <si>
-    <t>-0.3</t>
+    <t>3.4</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
RunnerHelperTrading rörig - dela upp
</commit_message>
<xml_diff>
--- a/src/main/java/safe_rl/runners/trading/results/scen_res_DayId[year=24, month=0, day=0, region=se3].xlsx
+++ b/src/main/java/safe_rl/runners/trading/results/scen_res_DayId[year=24, month=0, day=0, region=se3].xlsx
@@ -47,7 +47,7 @@
     <t>G2V</t>
   </si>
   <si>
-    <t>-5.3</t>
+    <t>-5.2</t>
   </si>
   <si>
     <t>-0</t>
@@ -56,13 +56,13 @@
     <t>V2G</t>
   </si>
   <si>
-    <t>3.9</t>
+    <t>2.5</t>
   </si>
   <si>
     <t>-0.5</t>
   </si>
   <si>
-    <t>3.4</t>
+    <t>2.0</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
HW cost från annuitet
</commit_message>
<xml_diff>
--- a/src/main/java/safe_rl/runners/trading/results/scen_res_DayId[year=24, month=0, day=0, region=se3].xlsx
+++ b/src/main/java/safe_rl/runners/trading/results/scen_res_DayId[year=24, month=0, day=0, region=se3].xlsx
@@ -47,7 +47,7 @@
     <t>G2V</t>
   </si>
   <si>
-    <t>-5.3</t>
+    <t>-5.4</t>
   </si>
   <si>
     <t>-0</t>
@@ -56,13 +56,13 @@
     <t>V2G</t>
   </si>
   <si>
-    <t>3.5</t>
-  </si>
-  <si>
-    <t>-0.5</t>
-  </si>
-  <si>
-    <t>3.0</t>
+    <t>4.8</t>
+  </si>
+  <si>
+    <t>-0.1</t>
+  </si>
+  <si>
+    <t>4.7</t>
   </si>
 </sst>
 </file>

</xml_diff>